<commit_message>
cleanup of unused files
</commit_message>
<xml_diff>
--- a/Figures/Table_1.xlsx
+++ b/Figures/Table_1.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Estimated Bounds Model" sheetId="4" r:id="rId6"/>
     <sheet name="Theoretical Bounds Model" sheetId="5" r:id="rId7"/>
     <sheet name="Weibull Model" sheetId="6" r:id="rId8"/>
+    <sheet name="Estimated Bounds Model v2" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="273">
   <si>
     <t>Var1</t>
   </si>
@@ -372,6 +373,315 @@
   </si>
   <si>
     <t>Sheffield</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>\lambda</t>
+  </si>
+  <si>
+    <t>\eta_{0}</t>
+  </si>
+  <si>
+    <t>d_{min}</t>
+  </si>
+  <si>
+    <t>d_{max}</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>All Cities</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Sheffield</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>England &amp; Wales 1848</t>
+  </si>
+  <si>
+    <t>England &amp; Wales 1890</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>\lambda</t>
+  </si>
+  <si>
+    <t>\eta_{0}</t>
+  </si>
+  <si>
+    <t>d_{min}</t>
+  </si>
+  <si>
+    <t>d_{max}</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>All Cities</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Sheffield</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>England &amp; Wales 1848</t>
+  </si>
+  <si>
+    <t>England &amp; Wales 1890</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>\lambda</t>
+  </si>
+  <si>
+    <t>\eta_{0}</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>All Cities</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Sheffield</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>England &amp; Wales 1848</t>
+  </si>
+  <si>
+    <t>England &amp; Wales 1890</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>\lambda</t>
+  </si>
+  <si>
+    <t>\eta_{0}</t>
+  </si>
+  <si>
+    <t>d_{min}</t>
+  </si>
+  <si>
+    <t>d_{max}</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>All Cities</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Sheffield</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>England &amp; Wales 1848</t>
+  </si>
+  <si>
+    <t>England &amp; Wales 1890</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>\lambda</t>
+  </si>
+  <si>
+    <t>\eta_{0}</t>
+  </si>
+  <si>
+    <t>d_{min}</t>
+  </si>
+  <si>
+    <t>d_{max}</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>All Cities</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Sheffield</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>\lambda</t>
+  </si>
+  <si>
+    <t>\eta_{0}</t>
+  </si>
+  <si>
+    <t>d_{min}</t>
+  </si>
+  <si>
+    <t>d_{max}</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>All Cities</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Sheffield</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>England &amp; Wales 1848</t>
+  </si>
+  <si>
+    <t>England &amp; Wales 1890</t>
   </si>
   <si>
     <t>Var1</t>
@@ -593,48 +903,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>91</v>
+        <v>176</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>92</v>
+        <v>177</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>93</v>
+        <v>178</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>94</v>
+        <v>179</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>96</v>
+        <v>181</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>97</v>
+        <v>182</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>98</v>
+        <v>183</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>99</v>
+        <v>184</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>100</v>
+        <v>185</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>101</v>
+        <v>186</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>102</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>86</v>
+        <v>171</v>
       </c>
       <c r="B2" s="0">
         <v>0.11600000000000001</v>
@@ -675,7 +985,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>87</v>
+        <v>172</v>
       </c>
       <c r="B3" s="0">
         <v>3.694</v>
@@ -716,7 +1026,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>88</v>
+        <v>173</v>
       </c>
       <c r="B4" s="0">
         <v>23.827999999999999</v>
@@ -757,7 +1067,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="B5" s="0">
         <v>3059.1900000000001</v>
@@ -798,7 +1108,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>90</v>
+        <v>175</v>
       </c>
       <c r="B6" s="0">
         <v>37</v>
@@ -860,39 +1170,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>103</v>
+        <v>188</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>109</v>
+        <v>194</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>110</v>
+        <v>195</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>111</v>
+        <v>196</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>112</v>
+        <v>197</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>113</v>
+        <v>198</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>114</v>
+        <v>199</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>115</v>
+        <v>200</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>116</v>
+        <v>201</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>117</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>104</v>
+        <v>189</v>
       </c>
       <c r="B2" s="0">
         <v>0.12</v>
@@ -924,7 +1234,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>105</v>
+        <v>190</v>
       </c>
       <c r="B3" s="0">
         <v>4.5800000000000001</v>
@@ -956,7 +1266,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>106</v>
+        <v>191</v>
       </c>
       <c r="B4" s="0">
         <v>11.664</v>
@@ -988,7 +1298,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>107</v>
+        <v>192</v>
       </c>
       <c r="B5" s="0">
         <v>4550</v>
@@ -1020,7 +1330,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>108</v>
+        <v>193</v>
       </c>
       <c r="B6" s="0">
         <v>37</v>
@@ -1076,48 +1386,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>118</v>
+        <v>203</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>124</v>
+        <v>209</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>125</v>
+        <v>210</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>126</v>
+        <v>211</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>127</v>
+        <v>212</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>128</v>
+        <v>213</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>129</v>
+        <v>214</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>130</v>
+        <v>215</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>131</v>
+        <v>216</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>133</v>
+        <v>218</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>134</v>
+        <v>219</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>135</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>119</v>
+        <v>204</v>
       </c>
       <c r="B2" s="0">
         <v>0.23899999999999999</v>
@@ -1126,7 +1436,7 @@
         <v>0.129</v>
       </c>
       <c r="D2" s="0">
-        <v>0.32500000000000001</v>
+        <v>0.64600000000000002</v>
       </c>
       <c r="E2" s="0">
         <v>0.218</v>
@@ -1135,7 +1445,7 @@
         <v>0.218</v>
       </c>
       <c r="G2" s="0">
-        <v>0.29999999999999999</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="H2" s="0">
         <v>0.27200000000000002</v>
@@ -1147,7 +1457,7 @@
         <v>0.24399999999999999</v>
       </c>
       <c r="K2" s="0">
-        <v>0.32300000000000001</v>
+        <v>0.624</v>
       </c>
       <c r="L2" s="0">
         <v>0.222</v>
@@ -1158,7 +1468,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>120</v>
+        <v>205</v>
       </c>
       <c r="B3" s="0">
         <v>7.9610000000000003</v>
@@ -1167,7 +1477,7 @@
         <v>4.5140000000000002</v>
       </c>
       <c r="D3" s="0">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E3" s="0">
         <v>7.0330000000000004</v>
@@ -1176,7 +1486,7 @@
         <v>7.0659999999999998</v>
       </c>
       <c r="G3" s="0">
-        <v>10</v>
+        <v>18.277999999999999</v>
       </c>
       <c r="H3" s="0">
         <v>9.0920000000000005</v>
@@ -1188,7 +1498,7 @@
         <v>8.891</v>
       </c>
       <c r="K3" s="0">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L3" s="0">
         <v>7.2160000000000002</v>
@@ -1199,7 +1509,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>121</v>
+        <v>206</v>
       </c>
       <c r="B4" s="0">
         <v>23.827999999999999</v>
@@ -1240,7 +1550,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>122</v>
+        <v>207</v>
       </c>
       <c r="B5" s="0">
         <v>765.21900000000005</v>
@@ -1281,7 +1591,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>123</v>
+        <v>208</v>
       </c>
       <c r="B6" s="0">
         <v>37</v>
@@ -1346,48 +1656,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>136</v>
+        <v>239</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>142</v>
+        <v>245</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>143</v>
+        <v>246</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>144</v>
+        <v>247</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>145</v>
+        <v>248</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>146</v>
+        <v>249</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>147</v>
+        <v>250</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>148</v>
+        <v>251</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>149</v>
+        <v>252</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>150</v>
+        <v>253</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>151</v>
+        <v>254</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>152</v>
+        <v>255</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>153</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>137</v>
+        <v>240</v>
       </c>
       <c r="B2" s="0">
         <v>0.035999999999999997</v>
@@ -1428,7 +1738,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>138</v>
+        <v>241</v>
       </c>
       <c r="B3" s="0">
         <v>2.7919999999999998</v>
@@ -1469,7 +1779,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>139</v>
+        <v>242</v>
       </c>
       <c r="B4" s="0">
         <v>1</v>
@@ -1510,7 +1820,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>140</v>
+        <v>243</v>
       </c>
       <c r="B5" s="0">
         <v>1000000</v>
@@ -1551,7 +1861,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>141</v>
+        <v>244</v>
       </c>
       <c r="B6" s="0">
         <v>37</v>
@@ -1616,48 +1926,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>154</v>
+        <v>257</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>158</v>
+        <v>261</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>159</v>
+        <v>262</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>160</v>
+        <v>263</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>161</v>
+        <v>264</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>162</v>
+        <v>265</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>163</v>
+        <v>266</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>164</v>
+        <v>267</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>165</v>
+        <v>268</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>166</v>
+        <v>269</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>167</v>
+        <v>270</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>168</v>
+        <v>271</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>169</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>155</v>
+        <v>258</v>
       </c>
       <c r="B2" s="0">
         <v>0.0060000000000000001</v>
@@ -1698,7 +2008,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>156</v>
+        <v>259</v>
       </c>
       <c r="B3" s="0">
         <v>0.94499999999999995</v>
@@ -1739,7 +2049,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>157</v>
+        <v>260</v>
       </c>
       <c r="B4" s="0">
         <v>37</v>
@@ -1775,6 +2085,276 @@
         <v>41</v>
       </c>
       <c r="M4" s="0">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" customWidth="true"/>
+    <col min="2" max="2" width="9" customWidth="true"/>
+    <col min="3" max="3" width="8.7109375" customWidth="true"/>
+    <col min="4" max="4" width="11.85546875" customWidth="true"/>
+    <col min="5" max="5" width="8.7109375" customWidth="true"/>
+    <col min="6" max="6" width="8.5703125" customWidth="true"/>
+    <col min="7" max="7" width="9.42578125" customWidth="true"/>
+    <col min="8" max="8" width="8.7109375" customWidth="true"/>
+    <col min="9" max="9" width="11.5703125" customWidth="true"/>
+    <col min="10" max="10" width="9.28515625" customWidth="true"/>
+    <col min="11" max="11" width="5.7109375" customWidth="true"/>
+    <col min="12" max="12" width="20.28515625" customWidth="true"/>
+    <col min="13" max="13" width="20.28515625" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0.123</v>
+      </c>
+      <c r="C2" s="0">
+        <v>0.082000000000000003</v>
+      </c>
+      <c r="D2" s="0">
+        <v>0.17000000000000001</v>
+      </c>
+      <c r="E2" s="0">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="F2" s="0">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="G2" s="0">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="H2" s="0">
+        <v>0.104</v>
+      </c>
+      <c r="I2" s="0">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J2" s="0">
+        <v>0.123</v>
+      </c>
+      <c r="K2" s="0">
+        <v>0.247</v>
+      </c>
+      <c r="L2" s="0">
+        <v>0.188</v>
+      </c>
+      <c r="M2" s="0">
+        <v>0.11700000000000001</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" s="0">
+        <v>4.1639999999999997</v>
+      </c>
+      <c r="C3" s="0">
+        <v>2.8919999999999999</v>
+      </c>
+      <c r="D3" s="0">
+        <v>5.4569999999999999</v>
+      </c>
+      <c r="E3" s="0">
+        <v>3.7879999999999998</v>
+      </c>
+      <c r="F3" s="0">
+        <v>4.9379999999999997</v>
+      </c>
+      <c r="G3" s="0">
+        <v>6.9720000000000004</v>
+      </c>
+      <c r="H3" s="0">
+        <v>3.52</v>
+      </c>
+      <c r="I3" s="0">
+        <v>4.8739999999999997</v>
+      </c>
+      <c r="J3" s="0">
+        <v>4.7039999999999997</v>
+      </c>
+      <c r="K3" s="0">
+        <v>7.9500000000000002</v>
+      </c>
+      <c r="L3" s="0">
+        <v>6.367</v>
+      </c>
+      <c r="M3" s="0">
+        <v>2.4049999999999998</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" s="0">
+        <v>23.827999999999999</v>
+      </c>
+      <c r="C4" s="0">
+        <v>21.977</v>
+      </c>
+      <c r="D4" s="0">
+        <v>26.841000000000001</v>
+      </c>
+      <c r="E4" s="0">
+        <v>24.937999999999999</v>
+      </c>
+      <c r="F4" s="0">
+        <v>24</v>
+      </c>
+      <c r="G4" s="0">
+        <v>19</v>
+      </c>
+      <c r="H4" s="0">
+        <v>23.117999999999999</v>
+      </c>
+      <c r="I4" s="0">
+        <v>23.088000000000001</v>
+      </c>
+      <c r="J4" s="0">
+        <v>11.664</v>
+      </c>
+      <c r="K4" s="0">
+        <v>14</v>
+      </c>
+      <c r="L4" s="0">
+        <v>2</v>
+      </c>
+      <c r="M4" s="0">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" s="0">
+        <v>3059.1900000000001</v>
+      </c>
+      <c r="C5" s="0">
+        <v>3643.7660000000001</v>
+      </c>
+      <c r="D5" s="0">
+        <v>2496.5520000000001</v>
+      </c>
+      <c r="E5" s="0">
+        <v>2671.0410000000002</v>
+      </c>
+      <c r="F5" s="0">
+        <v>1812</v>
+      </c>
+      <c r="G5" s="0">
+        <v>1775.0540000000001</v>
+      </c>
+      <c r="H5" s="0">
+        <v>4458.1490000000003</v>
+      </c>
+      <c r="I5" s="0">
+        <v>3066.9549999999999</v>
+      </c>
+      <c r="J5" s="0">
+        <v>4550</v>
+      </c>
+      <c r="K5" s="0">
+        <v>3018</v>
+      </c>
+      <c r="L5" s="0">
+        <v>459</v>
+      </c>
+      <c r="M5" s="0">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="0">
+        <v>37</v>
+      </c>
+      <c r="C6" s="0">
+        <v>27</v>
+      </c>
+      <c r="D6" s="0">
+        <v>28</v>
+      </c>
+      <c r="E6" s="0">
+        <v>36</v>
+      </c>
+      <c r="F6" s="0">
+        <v>37</v>
+      </c>
+      <c r="G6" s="0">
+        <v>37</v>
+      </c>
+      <c r="H6" s="0">
+        <v>35</v>
+      </c>
+      <c r="I6" s="0">
+        <v>36</v>
+      </c>
+      <c r="J6" s="0">
+        <v>37</v>
+      </c>
+      <c r="K6" s="0">
+        <v>37</v>
+      </c>
+      <c r="L6" s="0">
+        <v>41</v>
+      </c>
+      <c r="M6" s="0">
         <v>26</v>
       </c>
     </row>

</xml_diff>